<commit_message>
fixed versus and improved level layout
</commit_message>
<xml_diff>
--- a/Data/LevelLayout2.xlsx
+++ b/Data/LevelLayout2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saril\Documents\GitHub\Programming4\2DAE14_Janssen_Sari_Tron\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CBF888-5015-4AA5-9B29-8ACA68357AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A75D431-633E-4BD2-BB91-73CF8FE60D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DA9D7AD-EAE2-43E4-A737-467F9E8D8689}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:BF54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AT13" sqref="AT13"/>
+      <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4037,11 +4037,11 @@
       <c r="P21" s="4">
         <v>2</v>
       </c>
-      <c r="Q21" s="4">
-        <v>2</v>
-      </c>
-      <c r="R21" s="4">
-        <v>2</v>
+      <c r="Q21" s="7">
+        <v>5</v>
+      </c>
+      <c r="R21" s="7">
+        <v>5</v>
       </c>
       <c r="S21" s="4">
         <v>2</v>
@@ -4073,11 +4073,11 @@
       <c r="AB21" s="4">
         <v>2</v>
       </c>
-      <c r="AC21" s="7">
-        <v>5</v>
-      </c>
-      <c r="AD21" s="7">
-        <v>5</v>
+      <c r="AC21" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="4">
+        <v>2</v>
       </c>
       <c r="AE21" s="4">
         <v>2</v>
@@ -4213,11 +4213,11 @@
       <c r="P22" s="4">
         <v>2</v>
       </c>
-      <c r="Q22" s="4">
-        <v>2</v>
-      </c>
-      <c r="R22" s="4">
-        <v>2</v>
+      <c r="Q22" s="7">
+        <v>5</v>
+      </c>
+      <c r="R22" s="7">
+        <v>5</v>
       </c>
       <c r="S22" s="4">
         <v>2</v>
@@ -4249,11 +4249,11 @@
       <c r="AB22" s="4">
         <v>2</v>
       </c>
-      <c r="AC22" s="7">
-        <v>5</v>
-      </c>
-      <c r="AD22" s="7">
-        <v>5</v>
+      <c r="AC22" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD22" s="4">
+        <v>2</v>
       </c>
       <c r="AE22" s="4">
         <v>2</v>

</xml_diff>